<commit_message>
Fixed children calc;More speedups
</commit_message>
<xml_diff>
--- a/tables/extract_scores.xlsx
+++ b/tables/extract_scores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="7845"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="7848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,9 +342,9 @@
       <selection sqref="A1:Y109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>26</v>
       </c>
@@ -421,7 +421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>66</v>
       </c>
@@ -489,7 +489,7 @@
         <v>15</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X2">
         <v>5</v>
@@ -498,7 +498,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>19</v>
       </c>
@@ -575,7 +575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>66</v>
       </c>
@@ -652,7 +652,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>29</v>
       </c>
@@ -720,7 +720,7 @@
         <v>15</v>
       </c>
       <c r="W5">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X5">
         <v>15</v>
@@ -729,7 +729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>55</v>
       </c>
@@ -797,7 +797,7 @@
         <v>40</v>
       </c>
       <c r="W6">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X6">
         <v>30</v>
@@ -806,7 +806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>34</v>
       </c>
@@ -874,7 +874,7 @@
         <v>20</v>
       </c>
       <c r="W7">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -883,7 +883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>48</v>
       </c>
@@ -951,7 +951,7 @@
         <v>30</v>
       </c>
       <c r="W8">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X8">
         <v>30</v>
@@ -960,7 +960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>47</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X9">
         <v>10</v>
@@ -1037,7 +1037,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>59</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>45</v>
       </c>
       <c r="W10">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="X10">
         <v>40</v>
@@ -1114,7 +1114,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>21</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>51</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>35</v>
       </c>
       <c r="W12">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -1268,7 +1268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>53</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>40</v>
       </c>
       <c r="W13">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="X13">
         <v>5</v>
@@ -1345,7 +1345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>23</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>24</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>48</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>30</v>
       </c>
       <c r="W16">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X16">
         <v>20</v>
@@ -1576,7 +1576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>55</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X17">
         <v>5</v>
@@ -1653,7 +1653,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>20</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>22</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>71</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>65</v>
       </c>
       <c r="W20">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>65</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>25</v>
       </c>
       <c r="W21">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X21">
         <v>0</v>
@@ -1961,7 +1961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>52</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>73</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>22</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>30</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>69</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>15</v>
       </c>
       <c r="W29">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X29">
         <v>25</v>
@@ -2577,7 +2577,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>23</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>48</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="W31">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X31">
         <v>30</v>
@@ -2731,7 +2731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>20</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>22</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>70</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="W34">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X34">
         <v>15</v>
@@ -2962,7 +2962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>47</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>30</v>
       </c>
       <c r="W35">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X35">
         <v>10</v>
@@ -3039,7 +3039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>26</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>28</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>62</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>45</v>
       </c>
       <c r="W38">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X38">
         <v>25</v>
@@ -3270,7 +3270,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>72</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>40</v>
       </c>
       <c r="W39">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X39">
         <v>20</v>
@@ -3347,7 +3347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>22</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>28</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>25</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>65</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>50</v>
       </c>
       <c r="W43">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X43">
         <v>30</v>
@@ -3655,7 +3655,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>67</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>5</v>
       </c>
       <c r="W44">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="X44">
         <v>10</v>
@@ -3732,7 +3732,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>30</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>67</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="W46">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X46">
         <v>15</v>
@@ -3886,7 +3886,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>35</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>24</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>20</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>20</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>21</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>43</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="W52">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X52">
         <v>0</v>
@@ -4348,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>23</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>22</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>20</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>22</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="W56">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X56">
         <v>0</v>
@@ -4656,7 +4656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>31</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>69</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>30</v>
       </c>
       <c r="W58">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X58">
         <v>15</v>
@@ -4810,7 +4810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>68</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>55</v>
       </c>
       <c r="W59">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X59">
         <v>5</v>
@@ -4887,7 +4887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>65</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="W60">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X60">
         <v>30</v>
@@ -4964,7 +4964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>21</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>26</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>55</v>
       </c>
       <c r="W63">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X63">
         <v>45</v>
@@ -5195,7 +5195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>25</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>24</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>19</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>21</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>0</v>
       </c>
       <c r="W69">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X69">
         <v>0</v>
@@ -5657,7 +5657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>67</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>0</v>
       </c>
       <c r="W70">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X70">
         <v>0</v>
@@ -5734,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>42</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>25</v>
       </c>
       <c r="W71">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X71">
         <v>25</v>
@@ -5811,7 +5811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>52</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>35</v>
       </c>
       <c r="W72">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X72">
         <v>35</v>
@@ -5888,7 +5888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>56</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>40</v>
       </c>
       <c r="W73">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X73">
         <v>30</v>
@@ -5965,7 +5965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>32</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>51</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>35</v>
       </c>
       <c r="W75">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="X75">
         <v>15</v>
@@ -6119,7 +6119,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>49</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>15</v>
       </c>
       <c r="W76">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X76">
         <v>10</v>
@@ -6196,7 +6196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>43</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>25</v>
       </c>
       <c r="W77">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X77">
         <v>20</v>
@@ -6273,7 +6273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>22</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>20</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>0</v>
       </c>
       <c r="W79">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X79">
         <v>10</v>
@@ -6427,7 +6427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>45</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>30</v>
       </c>
       <c r="W80">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X80">
         <v>0</v>
@@ -6504,7 +6504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>23</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>18</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <v>49</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>35</v>
       </c>
       <c r="W83">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X83">
         <v>25</v>
@@ -6735,7 +6735,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>61</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>45</v>
       </c>
       <c r="W84">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X84">
         <v>5</v>
@@ -6812,7 +6812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>51</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>35</v>
       </c>
       <c r="W85">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X85">
         <v>0</v>
@@ -6889,7 +6889,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>35</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>10</v>
       </c>
       <c r="W86">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X86">
         <v>5</v>
@@ -6966,7 +6966,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>36</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>72</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <v>32</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>55</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>40</v>
       </c>
       <c r="W90">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X90">
         <v>0</v>
@@ -7274,7 +7274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
         <v>75</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>15</v>
       </c>
       <c r="W91">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="X91">
         <v>50</v>
@@ -7351,7 +7351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <v>44</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>30</v>
       </c>
       <c r="W92">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X92">
         <v>0</v>
@@ -7428,7 +7428,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
         <v>56</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>40</v>
       </c>
       <c r="W93">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X93">
         <v>15</v>
@@ -7505,7 +7505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>61</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
         <v>24</v>
       </c>
@@ -7659,7 +7659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <v>55</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>30</v>
       </c>
       <c r="W96">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X96">
         <v>25</v>
@@ -7736,7 +7736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <v>59</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>45</v>
       </c>
       <c r="W97">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X97">
         <v>25</v>
@@ -7813,7 +7813,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <v>38</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
         <v>21</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>72</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <v>63</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>45</v>
       </c>
       <c r="W101">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X101">
         <v>0</v>
@@ -8121,7 +8121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <v>31</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <v>61</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>45</v>
       </c>
       <c r="W103">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X103">
         <v>30</v>
@@ -8275,7 +8275,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <v>67</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>50</v>
       </c>
       <c r="W104">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X104">
         <v>0</v>
@@ -8352,7 +8352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
         <v>22</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A106">
         <v>54</v>
       </c>
@@ -8497,7 +8497,7 @@
         <v>40</v>
       </c>
       <c r="W106">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X106">
         <v>0</v>
@@ -8506,7 +8506,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A107">
         <v>63</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>45</v>
       </c>
       <c r="W107">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="X107">
         <v>35</v>
@@ -8583,7 +8583,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A108">
         <v>24</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A109">
         <v>53</v>
       </c>
@@ -8728,7 +8728,7 @@
         <v>35</v>
       </c>
       <c r="W109">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="X109">
         <v>0</v>
@@ -8737,7 +8737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A110">
         <v>53</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A111">
         <v>64</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A112">
         <v>25</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A113">
         <v>24</v>
       </c>
@@ -9045,7 +9045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A114">
         <v>19</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A115">
         <v>21</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A116">
         <v>67</v>
       </c>
@@ -9276,7 +9276,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A117">
         <v>67</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A118">
         <v>42</v>
       </c>
@@ -9430,7 +9430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A119">
         <v>52</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A120">
         <v>56</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A121">
         <v>32</v>
       </c>
@@ -9661,7 +9661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A122">
         <v>51</v>
       </c>
@@ -9738,7 +9738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A123">
         <v>49</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A124">
         <v>43</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A125">
         <v>22</v>
       </c>
@@ -9969,7 +9969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A126">
         <v>20</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A127">
         <v>45</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A128">
         <v>23</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A129">
         <v>18</v>
       </c>
@@ -10277,7 +10277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A130">
         <v>49</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A131">
         <v>61</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A132">
         <v>51</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A133">
         <v>58</v>
       </c>
@@ -10585,7 +10585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A134">
         <v>54</v>
       </c>
@@ -10662,7 +10662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A135">
         <v>35</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A136">
         <v>72</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A137">
         <v>32</v>
       </c>
@@ -10893,7 +10893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A138">
         <v>55</v>
       </c>
@@ -10970,7 +10970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A139">
         <v>75</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A140">
         <v>44</v>
       </c>
@@ -11124,7 +11124,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A141">
         <v>56</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A142">
         <v>61</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A143">
         <v>24</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A144">
         <v>55</v>
       </c>
@@ -11432,7 +11432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A145">
         <v>59</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A146">
         <v>38</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A147">
         <v>75</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A148">
         <v>79</v>
       </c>
@@ -11740,7 +11740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A149">
         <v>61</v>
       </c>
@@ -11817,7 +11817,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A150">
         <v>54</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A151">
         <v>64</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A152">
         <v>63</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A153">
         <v>64</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A154">
         <v>21</v>
       </c>
@@ -12202,7 +12202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A155">
         <v>72</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A156">
         <v>63</v>
       </c>
@@ -12356,7 +12356,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A157">
         <v>31</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A158">
         <v>31</v>
       </c>
@@ -12510,7 +12510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A159">
         <v>24</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A160">
         <v>61</v>
       </c>
@@ -12664,7 +12664,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A161">
         <v>67</v>
       </c>
@@ -12741,7 +12741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A162">
         <v>26</v>
       </c>
@@ -12818,7 +12818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A163">
         <v>22</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A164">
         <v>54</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A165">
         <v>63</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A166">
         <v>24</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A167">
         <v>53</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A168">
         <v>68</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A169">
         <v>28</v>
       </c>
@@ -13357,7 +13357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A170">
         <v>64</v>
       </c>
@@ -13434,7 +13434,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A171">
         <v>40</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A172">
         <v>55</v>
       </c>
@@ -13588,7 +13588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A173">
         <v>21</v>
       </c>
@@ -13665,7 +13665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A174">
         <v>54</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A175">
         <v>63</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A176">
         <v>24</v>
       </c>
@@ -13896,7 +13896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A177">
         <v>53</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A178">
         <v>68</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A179">
         <v>28</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A180">
         <v>64</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A181">
         <v>40</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A182">
         <v>55</v>
       </c>
@@ -14358,7 +14358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A183">
         <v>21</v>
       </c>
@@ -14435,7 +14435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A184">
         <v>28</v>
       </c>
@@ -14512,7 +14512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A185">
         <v>64</v>
       </c>
@@ -14589,7 +14589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A186">
         <v>40</v>
       </c>
@@ -14666,7 +14666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A187">
         <v>55</v>
       </c>
@@ -14743,7 +14743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A188">
         <v>21</v>
       </c>

</xml_diff>